<commit_message>
update export ticket finish
</commit_message>
<xml_diff>
--- a/public/Ticket Approval.xlsx
+++ b/public/Ticket Approval.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\imirs\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\i-mirs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692FD0DF-343D-4F9D-B698-BDB255CE8D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46CDA9D-71F8-422E-828C-4B0365DE3C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet Export" sheetId="3" r:id="rId1"/>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,11 +200,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -232,43 +227,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -343,6 +301,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -355,41 +328,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -916,7 +876,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D8" sqref="D8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -935,169 +895,169 @@
   <sheetData>
     <row r="1" spans="1:7" ht="7.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" ht="5.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="14" t="str">
         <f>'Sheet Export'!A2</f>
         <v>2023-04-10 11:09:33.000</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="10"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="14" t="str">
         <f>'Sheet Export'!E2</f>
         <v>RE20230410001</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="14">
         <f>'Sheet Export'!I2</f>
         <v>11480</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>'Sheet Export'!H2</f>
         <v>RCY OP 60</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="10"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="str">
+      <c r="D8" s="14" t="str">
         <f>'Sheet Export'!K2</f>
         <v>SPROCKET LADLE DCM 7</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="10"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="14" t="str">
         <f>'Sheet Export'!L2</f>
         <v>Y003999 [DRAWING]</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="14" t="str">
         <f>'Sheet Export'!N2</f>
         <v>qwewqe</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="14">
         <f>'Sheet Export'!M2</f>
         <v>15</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="10"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="14" t="str">
         <f>'Sheet Export'!O2</f>
         <v>qweqwe</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="14" t="str">
         <f>'Sheet Export'!P2</f>
         <v>Riko</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="10"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>